<commit_message>
data: update structure info table
</commit_message>
<xml_diff>
--- a/data/PDB_structure_info.xlsx
+++ b/data/PDB_structure_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikkelrasmussen/Library/CloudStorage/OneDrive-DanmarksTekniskeUniversitet/DTU/Bioinformatics_and_Systems_Biology/2_semester/Protein structure and computational biology (22117)/22117-PSCB-final-project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s193518_dtu_dk/Documents/DTU/Bioinformatics_and_Systems_Biology/2_semester/Protein structure and computational biology (22117)/22117-PSCB-final-project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50D95E4-5A81-DF4C-BF7E-4DCD6E4729B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{A50D95E4-5A81-DF4C-BF7E-4DCD6E4729B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{072250F3-C3C0-D345-982B-30AEE48756E3}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,6 +440,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -477,11 +485,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,7 +796,7 @@
   <dimension ref="A1:M68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -850,124 +859,100 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="G2">
-        <v>0.192</v>
-      </c>
-      <c r="H2">
-        <v>0.192</v>
-      </c>
       <c r="I2">
-        <v>1997</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>5.29</v>
-      </c>
-      <c r="L2">
-        <v>1.42</v>
-      </c>
-      <c r="M2">
-        <v>1.1499999999999999</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="G3">
-        <v>0.192</v>
-      </c>
-      <c r="H3">
-        <v>0.192</v>
-      </c>
       <c r="I3">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="K3">
-        <v>5.64</v>
-      </c>
-      <c r="L3">
-        <v>3.32</v>
+        <v>30.64</v>
       </c>
       <c r="M3">
-        <v>0.57999999999999996</v>
+        <v>18.670000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>82</v>
+      </c>
+      <c r="F4">
+        <v>0.21329999999999999</v>
       </c>
       <c r="G4">
-        <v>0.19800000000000001</v>
+        <v>0.18</v>
       </c>
       <c r="H4">
-        <v>0.19800000000000001</v>
+        <v>0.18179999999999999</v>
       </c>
       <c r="I4">
-        <v>1997</v>
+        <v>2021</v>
       </c>
       <c r="J4">
-        <v>0.49</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>3.51</v>
+        <v>0.9</v>
       </c>
       <c r="L4">
-        <v>4.76</v>
+        <v>6.57</v>
       </c>
       <c r="M4">
-        <v>2.82</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -976,144 +961,141 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>110</v>
+      </c>
+      <c r="F5">
+        <v>0.22625999999999999</v>
       </c>
       <c r="G5">
-        <v>0.19800000000000001</v>
+        <v>0.18717</v>
       </c>
       <c r="H5">
-        <v>0.19800000000000001</v>
+        <v>0.18912000000000001</v>
       </c>
       <c r="I5">
-        <v>1997</v>
+        <v>2019</v>
       </c>
       <c r="J5">
-        <v>0.97</v>
+        <v>2.08</v>
       </c>
       <c r="K5">
-        <v>5.26</v>
+        <v>4.42</v>
+      </c>
+      <c r="L5">
+        <v>8.11</v>
       </c>
       <c r="M5">
-        <v>0.56000000000000005</v>
+        <v>2.34</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="G6">
-        <v>0.17399999999999999</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="H6">
-        <v>0.17399999999999999</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="I6">
-        <v>1997</v>
+        <v>2003</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>4.5</v>
-      </c>
-      <c r="L6">
-        <v>3.79</v>
+        <v>8.4700000000000006</v>
       </c>
       <c r="M6">
-        <v>1.17</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="G7">
-        <v>0.186</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="H7">
-        <v>0.186</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="I7">
-        <v>1997</v>
+        <v>2003</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <v>5.96</v>
-      </c>
-      <c r="L7">
-        <v>1.9</v>
+        <v>10.16</v>
       </c>
       <c r="M7">
-        <v>1.1599999999999999</v>
+        <v>6.45</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="G8">
-        <v>0.192</v>
+        <v>0.19</v>
       </c>
       <c r="H8">
-        <v>0.192</v>
+        <v>0.19</v>
       </c>
       <c r="I8">
-        <v>1997</v>
+        <v>2003</v>
       </c>
       <c r="J8">
-        <v>0.49</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>8.65</v>
-      </c>
-      <c r="L8">
-        <v>0.95</v>
+        <v>1.76</v>
       </c>
       <c r="M8">
-        <v>1.75</v>
+        <v>7.61</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>26</v>
+      <c r="A9" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
@@ -1128,82 +1110,103 @@
         <v>29</v>
       </c>
       <c r="F9">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="G9">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="H9">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="I9">
+        <v>1999</v>
+      </c>
+      <c r="J9">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="K9">
+        <v>15.55</v>
+      </c>
+      <c r="M9">
+        <v>12.37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10">
         <v>0.26400000000000001</v>
       </c>
-      <c r="G9">
+      <c r="G10">
         <v>0.21</v>
       </c>
-      <c r="H9">
+      <c r="H10">
         <v>0.21</v>
       </c>
-      <c r="I9">
+      <c r="I10">
         <v>1997</v>
       </c>
-      <c r="J9">
+      <c r="J10">
         <v>0.46</v>
       </c>
-      <c r="K9">
+      <c r="K10">
         <v>10.33</v>
       </c>
-      <c r="M9">
+      <c r="M10">
         <v>9.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10">
-        <v>1995</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>39</v>
+      </c>
+      <c r="G11">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="H11">
+        <v>0.19400000000000001</v>
       </c>
       <c r="I11">
-        <v>1995</v>
-      </c>
-      <c r="J11">
-        <v>2.5299999999999998</v>
+        <v>2003</v>
       </c>
       <c r="K11">
-        <v>30.64</v>
+        <v>12.41</v>
       </c>
       <c r="M11">
-        <v>18.670000000000002</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
@@ -1212,36 +1215,33 @@
         <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12">
-        <v>0.29399999999999998</v>
+        <v>39</v>
       </c>
       <c r="G12">
-        <v>0.23100000000000001</v>
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="H12">
+        <v>0.19900000000000001</v>
       </c>
       <c r="I12">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="J12">
-        <v>2.46</v>
+        <v>0.97</v>
       </c>
       <c r="K12">
-        <v>27.08</v>
-      </c>
-      <c r="L12">
-        <v>5.79</v>
+        <v>17.71</v>
       </c>
       <c r="M12">
-        <v>10.59</v>
+        <v>6.52</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
@@ -1250,33 +1250,39 @@
         <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>106</v>
+      </c>
+      <c r="F13">
+        <v>0.2303</v>
       </c>
       <c r="G13">
-        <v>0.20899999999999999</v>
+        <v>0.1981</v>
       </c>
       <c r="H13">
-        <v>0.20899999999999999</v>
+        <v>0.1996</v>
       </c>
       <c r="I13">
-        <v>2003</v>
+        <v>2012</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13">
-        <v>7.56</v>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="L13">
+        <v>6.48</v>
       </c>
       <c r="M13">
-        <v>4.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -1288,10 +1294,10 @@
         <v>39</v>
       </c>
       <c r="G14">
-        <v>0.192</v>
+        <v>0.193</v>
       </c>
       <c r="H14">
-        <v>0.192</v>
+        <v>0.193</v>
       </c>
       <c r="I14">
         <v>2003</v>
@@ -1300,18 +1306,18 @@
         <v>0</v>
       </c>
       <c r="K14">
-        <v>7.89</v>
+        <v>1.75</v>
       </c>
       <c r="M14">
-        <v>3.23</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
@@ -1323,10 +1329,10 @@
         <v>39</v>
       </c>
       <c r="G15">
-        <v>0.19600000000000001</v>
+        <v>0.19</v>
       </c>
       <c r="H15">
-        <v>0.19600000000000001</v>
+        <v>0.19</v>
       </c>
       <c r="I15">
         <v>2003</v>
@@ -1335,18 +1341,18 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <v>8.4700000000000006</v>
+        <v>3.54</v>
       </c>
       <c r="M15">
-        <v>2.15</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
@@ -1358,10 +1364,10 @@
         <v>39</v>
       </c>
       <c r="G16">
-        <v>0.19</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="H16">
-        <v>0.19</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="I16">
         <v>2003</v>
@@ -1370,18 +1376,18 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <v>10.69</v>
+        <v>11.72</v>
       </c>
       <c r="M16">
-        <v>3.23</v>
+        <v>6.45</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
@@ -1393,10 +1399,10 @@
         <v>39</v>
       </c>
       <c r="G17">
-        <v>0.2</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="H17">
-        <v>0.2</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="I17">
         <v>2003</v>
@@ -1405,18 +1411,18 @@
         <v>0</v>
       </c>
       <c r="K17">
-        <v>9.58</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="M17">
-        <v>3.23</v>
+        <v>5.43</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
         <v>15</v>
@@ -1428,10 +1434,10 @@
         <v>39</v>
       </c>
       <c r="G18">
-        <v>0.192</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="H18">
-        <v>0.192</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="I18">
         <v>2003</v>
@@ -1440,7 +1446,7 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <v>13.46</v>
+        <v>7.56</v>
       </c>
       <c r="M18">
         <v>4.3</v>
@@ -1448,10 +1454,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
         <v>15</v>
@@ -1475,18 +1481,18 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <v>4.51</v>
+        <v>7.89</v>
       </c>
       <c r="M19">
-        <v>2.15</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
         <v>15</v>
@@ -1498,19 +1504,22 @@
         <v>39</v>
       </c>
       <c r="G20">
-        <v>0.19400000000000001</v>
+        <v>0.19</v>
       </c>
       <c r="H20">
-        <v>0.19400000000000001</v>
+        <v>0.19</v>
       </c>
       <c r="I20">
         <v>2003</v>
       </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
       <c r="K20">
-        <v>12.41</v>
+        <v>10.69</v>
       </c>
       <c r="M20">
-        <v>4.3</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -1550,10 +1559,10 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
         <v>15</v>
@@ -1565,10 +1574,10 @@
         <v>39</v>
       </c>
       <c r="G22">
-        <v>0.20200000000000001</v>
+        <v>0.187</v>
       </c>
       <c r="H22">
-        <v>0.20200000000000001</v>
+        <v>0.187</v>
       </c>
       <c r="I22">
         <v>2003</v>
@@ -1577,18 +1586,18 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <v>10.16</v>
+        <v>11.43</v>
       </c>
       <c r="M22">
-        <v>6.45</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
         <v>15</v>
@@ -1600,10 +1609,10 @@
         <v>39</v>
       </c>
       <c r="G23">
-        <v>0.19600000000000001</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="H23">
-        <v>0.19600000000000001</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="I23">
         <v>2003</v>
@@ -1612,18 +1621,18 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>15.14</v>
+        <v>12.7</v>
       </c>
       <c r="M23">
-        <v>3.23</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
@@ -1635,10 +1644,10 @@
         <v>39</v>
       </c>
       <c r="G24">
-        <v>0.17699999999999999</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="H24">
-        <v>0.17699999999999999</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="I24">
         <v>2003</v>
@@ -1647,18 +1656,18 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <v>4.1399999999999997</v>
+        <v>5.23</v>
       </c>
       <c r="M24">
-        <v>7.69</v>
+        <v>7.53</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="C25" t="s">
         <v>15</v>
@@ -1667,33 +1676,39 @@
         <v>28</v>
       </c>
       <c r="E25" t="s">
-        <v>39</v>
+        <v>106</v>
+      </c>
+      <c r="F25">
+        <v>0.24610000000000001</v>
       </c>
       <c r="G25">
-        <v>0.17599999999999999</v>
+        <v>0.20449999999999999</v>
       </c>
       <c r="H25">
-        <v>0.17599999999999999</v>
+        <v>0.2064</v>
       </c>
       <c r="I25">
-        <v>2003</v>
+        <v>2012</v>
       </c>
       <c r="J25">
         <v>0</v>
       </c>
       <c r="K25">
-        <v>7.64</v>
+        <v>3.49</v>
+      </c>
+      <c r="L25">
+        <v>4.63</v>
       </c>
       <c r="M25">
-        <v>3.26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
         <v>15</v>
@@ -1705,10 +1720,10 @@
         <v>39</v>
       </c>
       <c r="G26">
-        <v>0.185</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="H26">
-        <v>0.185</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="I26">
         <v>2003</v>
@@ -1717,53 +1732,59 @@
         <v>0</v>
       </c>
       <c r="K26">
-        <v>8.7200000000000006</v>
+        <v>10.94</v>
       </c>
       <c r="M26">
-        <v>5.38</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
         <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>39</v>
+        <v>96</v>
+      </c>
+      <c r="F27">
+        <v>0.21190000000000001</v>
       </c>
       <c r="G27">
-        <v>0.16400000000000001</v>
+        <v>0.1656</v>
       </c>
       <c r="H27">
-        <v>0.16400000000000001</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="I27">
-        <v>2003</v>
+        <v>2012</v>
       </c>
       <c r="J27">
         <v>0</v>
       </c>
       <c r="K27">
-        <v>12.27</v>
+        <v>5.92</v>
+      </c>
+      <c r="L27">
+        <v>4.8600000000000003</v>
       </c>
       <c r="M27">
-        <v>4.4000000000000004</v>
+        <v>2.5099999999999998</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
         <v>15</v>
@@ -1772,33 +1793,39 @@
         <v>28</v>
       </c>
       <c r="E28" t="s">
-        <v>39</v>
+        <v>106</v>
+      </c>
+      <c r="F28">
+        <v>0.24510000000000001</v>
       </c>
       <c r="G28">
-        <v>0.19900000000000001</v>
+        <v>0.20519999999999999</v>
       </c>
       <c r="H28">
-        <v>0.19900000000000001</v>
+        <v>0.2072</v>
       </c>
       <c r="I28">
-        <v>2003</v>
+        <v>2012</v>
       </c>
       <c r="J28">
-        <v>0.97</v>
+        <v>0</v>
       </c>
       <c r="K28">
-        <v>17.71</v>
+        <v>2.9</v>
+      </c>
+      <c r="L28">
+        <v>7.41</v>
       </c>
       <c r="M28">
-        <v>6.52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
         <v>15</v>
@@ -1810,10 +1837,10 @@
         <v>39</v>
       </c>
       <c r="G29">
-        <v>0.156</v>
+        <v>0.2</v>
       </c>
       <c r="H29">
-        <v>0.156</v>
+        <v>0.2</v>
       </c>
       <c r="I29">
         <v>2003</v>
@@ -1822,18 +1849,18 @@
         <v>0</v>
       </c>
       <c r="K29">
-        <v>13.36</v>
+        <v>9.58</v>
       </c>
       <c r="M29">
-        <v>7.53</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
         <v>15</v>
@@ -1845,10 +1872,10 @@
         <v>39</v>
       </c>
       <c r="G30">
-        <v>0.20699999999999999</v>
+        <v>0.192</v>
       </c>
       <c r="H30">
-        <v>0.20699999999999999</v>
+        <v>0.192</v>
       </c>
       <c r="I30">
         <v>2003</v>
@@ -1857,18 +1884,18 @@
         <v>0</v>
       </c>
       <c r="K30">
-        <v>10.94</v>
+        <v>4.51</v>
       </c>
       <c r="M30">
-        <v>4.3</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C31" t="s">
         <v>15</v>
@@ -1880,10 +1907,10 @@
         <v>39</v>
       </c>
       <c r="G31">
-        <v>0.187</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="H31">
-        <v>0.187</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="I31">
         <v>2003</v>
@@ -1892,18 +1919,18 @@
         <v>0</v>
       </c>
       <c r="K31">
-        <v>11.43</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="M31">
-        <v>3.23</v>
+        <v>7.69</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
         <v>15</v>
@@ -1915,10 +1942,10 @@
         <v>39</v>
       </c>
       <c r="G32">
-        <v>0.193</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="H32">
-        <v>0.193</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="I32">
         <v>2003</v>
@@ -1927,18 +1954,18 @@
         <v>0</v>
       </c>
       <c r="K32">
-        <v>1.75</v>
+        <v>15.14</v>
       </c>
       <c r="M32">
-        <v>1.08</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
         <v>15</v>
@@ -1950,10 +1977,10 @@
         <v>39</v>
       </c>
       <c r="G33">
-        <v>0.19800000000000001</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="H33">
-        <v>0.19800000000000001</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="I33">
         <v>2003</v>
@@ -1962,18 +1989,18 @@
         <v>0</v>
       </c>
       <c r="K33">
-        <v>8.8000000000000007</v>
+        <v>7.64</v>
       </c>
       <c r="M33">
-        <v>5.43</v>
+        <v>3.26</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C34" t="s">
         <v>15</v>
@@ -1985,10 +2012,10 @@
         <v>39</v>
       </c>
       <c r="G34">
-        <v>0.19</v>
+        <v>0.16900000000000001</v>
       </c>
       <c r="H34">
-        <v>0.19</v>
+        <v>0.16900000000000001</v>
       </c>
       <c r="I34">
         <v>2003</v>
@@ -1997,18 +2024,18 @@
         <v>0</v>
       </c>
       <c r="K34">
-        <v>3.54</v>
+        <v>8.2200000000000006</v>
       </c>
       <c r="M34">
-        <v>2.17</v>
+        <v>5.43</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>69</v>
+      <c r="A35" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
         <v>15</v>
@@ -2017,103 +2044,118 @@
         <v>28</v>
       </c>
       <c r="E35" t="s">
-        <v>39</v>
+        <v>29</v>
+      </c>
+      <c r="F35">
+        <v>0.21340000000000001</v>
       </c>
       <c r="G35">
-        <v>0.20899999999999999</v>
+        <v>0.18781</v>
       </c>
       <c r="H35">
-        <v>0.20899999999999999</v>
+        <v>0.18909000000000001</v>
       </c>
       <c r="I35">
-        <v>2003</v>
+        <v>2005</v>
       </c>
       <c r="J35">
-        <v>0</v>
+        <v>0.22</v>
       </c>
       <c r="K35">
-        <v>11.72</v>
+        <v>1.8</v>
+      </c>
+      <c r="L35">
+        <v>5.97</v>
       </c>
       <c r="M35">
-        <v>6.45</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="C36" t="s">
         <v>15</v>
       </c>
       <c r="D36" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E36" t="s">
-        <v>39</v>
+        <v>82</v>
+      </c>
+      <c r="F36">
+        <v>0.25811000000000001</v>
       </c>
       <c r="G36">
-        <v>0.20200000000000001</v>
+        <v>0.21403</v>
       </c>
       <c r="H36">
-        <v>0.20200000000000001</v>
+        <v>0.2162</v>
       </c>
       <c r="I36">
-        <v>2003</v>
+        <v>2005</v>
       </c>
       <c r="J36">
         <v>0</v>
       </c>
       <c r="K36">
-        <v>12.7</v>
+        <v>5.26</v>
       </c>
       <c r="M36">
-        <v>4.3</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="C37" t="s">
         <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E37" t="s">
-        <v>39</v>
+        <v>110</v>
+      </c>
+      <c r="F37">
+        <v>0.1925</v>
       </c>
       <c r="G37">
-        <v>0.16900000000000001</v>
+        <v>0.1391</v>
       </c>
       <c r="H37">
-        <v>0.16900000000000001</v>
+        <v>0.14449999999999999</v>
       </c>
       <c r="I37">
-        <v>2003</v>
+        <v>2013</v>
       </c>
       <c r="J37">
         <v>0</v>
       </c>
       <c r="K37">
-        <v>8.2200000000000006</v>
+        <v>2.77</v>
+      </c>
+      <c r="L37">
+        <v>2.46</v>
       </c>
       <c r="M37">
-        <v>5.43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C38" t="s">
         <v>15</v>
@@ -2125,10 +2167,10 @@
         <v>39</v>
       </c>
       <c r="G38">
-        <v>0.17899999999999999</v>
+        <v>0.192</v>
       </c>
       <c r="H38">
-        <v>0.17899999999999999</v>
+        <v>0.192</v>
       </c>
       <c r="I38">
         <v>2003</v>
@@ -2137,18 +2179,18 @@
         <v>0</v>
       </c>
       <c r="K38">
-        <v>5.23</v>
+        <v>13.46</v>
       </c>
       <c r="M38">
-        <v>7.53</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C39" t="s">
         <v>15</v>
@@ -2160,10 +2202,10 @@
         <v>39</v>
       </c>
       <c r="G39">
-        <v>0.19</v>
+        <v>0.185</v>
       </c>
       <c r="H39">
-        <v>0.19</v>
+        <v>0.185</v>
       </c>
       <c r="I39">
         <v>2003</v>
@@ -2172,15 +2214,15 @@
         <v>0</v>
       </c>
       <c r="K39">
-        <v>1.76</v>
+        <v>8.7200000000000006</v>
       </c>
       <c r="M39">
-        <v>7.61</v>
+        <v>5.38</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
         <v>20</v>
@@ -2192,71 +2234,68 @@
         <v>28</v>
       </c>
       <c r="E40" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="G40">
-        <v>0.192</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="H40">
-        <v>0.192</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="I40">
-        <v>1994</v>
+        <v>2003</v>
       </c>
       <c r="J40">
-        <v>1.01</v>
+        <v>0</v>
       </c>
       <c r="K40">
-        <v>5.27</v>
+        <v>12.27</v>
       </c>
       <c r="M40">
-        <v>15.22</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="C41" t="s">
         <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E41" t="s">
-        <v>29</v>
-      </c>
-      <c r="F41">
-        <v>0.21340000000000001</v>
+        <v>17</v>
       </c>
       <c r="G41">
-        <v>0.18781</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="H41">
-        <v>0.18909000000000001</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="I41">
-        <v>2005</v>
+        <v>1997</v>
       </c>
       <c r="J41">
-        <v>0.22</v>
+        <v>0.49</v>
       </c>
       <c r="K41">
-        <v>1.8</v>
+        <v>3.51</v>
       </c>
       <c r="L41">
-        <v>5.97</v>
+        <v>4.76</v>
       </c>
       <c r="M41">
-        <v>1.3</v>
+        <v>2.82</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
         <v>20</v>
@@ -2268,71 +2307,68 @@
         <v>16</v>
       </c>
       <c r="E42" t="s">
-        <v>79</v>
-      </c>
-      <c r="F42">
-        <v>0.252</v>
+        <v>17</v>
       </c>
       <c r="G42">
-        <v>0.216</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="H42">
-        <v>0.216</v>
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="I42">
+        <v>1997</v>
       </c>
       <c r="J42">
-        <v>1.1000000000000001</v>
+        <v>0.97</v>
       </c>
       <c r="K42">
-        <v>4.97</v>
+        <v>5.26</v>
       </c>
       <c r="M42">
-        <v>5.51</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="C43" t="s">
         <v>15</v>
       </c>
       <c r="D43" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E43" t="s">
-        <v>82</v>
-      </c>
-      <c r="F43">
-        <v>0.25811000000000001</v>
+        <v>17</v>
       </c>
       <c r="G43">
-        <v>0.21403</v>
+        <v>0.192</v>
       </c>
       <c r="H43">
-        <v>0.2162</v>
+        <v>0.192</v>
       </c>
       <c r="I43">
-        <v>2005</v>
+        <v>1994</v>
       </c>
       <c r="J43">
-        <v>0</v>
+        <v>1.01</v>
       </c>
       <c r="K43">
-        <v>5.26</v>
+        <v>5.27</v>
       </c>
       <c r="M43">
-        <v>2.78</v>
+        <v>15.22</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="C44" t="s">
         <v>15</v>
@@ -2341,71 +2377,71 @@
         <v>16</v>
       </c>
       <c r="E44" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F44">
-        <v>0.24746000000000001</v>
+        <v>0.252</v>
       </c>
       <c r="G44">
-        <v>0.19312000000000001</v>
+        <v>0.216</v>
       </c>
       <c r="H44">
-        <v>0.19585</v>
-      </c>
-      <c r="I44">
-        <v>2005</v>
+        <v>0.216</v>
       </c>
       <c r="J44">
-        <v>0.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K44">
-        <v>4.1100000000000003</v>
+        <v>4.97</v>
       </c>
       <c r="M44">
-        <v>3.85</v>
+        <v>5.51</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C45" t="s">
         <v>15</v>
       </c>
       <c r="D45" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
       <c r="E45" t="s">
-        <v>82</v>
+        <v>126</v>
       </c>
       <c r="F45">
-        <v>0.31322</v>
+        <v>0.23860000000000001</v>
       </c>
       <c r="G45">
-        <v>0.21704000000000001</v>
+        <v>0.18429999999999999</v>
       </c>
       <c r="H45">
-        <v>0.22187000000000001</v>
+        <v>0.187</v>
       </c>
       <c r="I45">
-        <v>2005</v>
+        <v>2020</v>
       </c>
       <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>3.96</v>
+      </c>
+      <c r="L45">
         <v>2.14</v>
       </c>
-      <c r="K45">
-        <v>9.17</v>
-      </c>
       <c r="M45">
-        <v>12.5</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
         <v>88</v>
@@ -2417,311 +2453,308 @@
         <v>16</v>
       </c>
       <c r="E46" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F46">
-        <v>0.27100000000000002</v>
+        <v>0.25369999999999998</v>
       </c>
       <c r="G46">
-        <v>0.20599999999999999</v>
+        <v>0.21029999999999999</v>
+      </c>
+      <c r="H46">
+        <v>0.21240000000000001</v>
       </c>
       <c r="I46">
-        <v>2006</v>
+        <v>2014</v>
       </c>
       <c r="J46">
-        <v>0.77</v>
+        <v>0.19</v>
       </c>
       <c r="K46">
-        <v>13.88</v>
+        <v>7.28</v>
+      </c>
+      <c r="L46">
+        <v>6.04</v>
       </c>
       <c r="M46">
-        <v>4.1900000000000004</v>
+        <v>6.74</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C47" t="s">
         <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E47" t="s">
         <v>89</v>
       </c>
       <c r="F47">
-        <v>0.27700000000000002</v>
+        <v>0.27100000000000002</v>
       </c>
       <c r="G47">
-        <v>0.158</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="I47">
         <v>2006</v>
       </c>
       <c r="J47">
-        <v>1.2</v>
+        <v>0.77</v>
       </c>
       <c r="K47">
-        <v>18.739999999999998</v>
+        <v>13.88</v>
       </c>
       <c r="M47">
-        <v>4.09</v>
+        <v>4.1900000000000004</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" t="s">
+        <v>122</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" t="s">
+        <v>123</v>
+      </c>
+      <c r="E48" t="s">
+        <v>79</v>
+      </c>
+      <c r="F48">
+        <v>0.28489999999999999</v>
+      </c>
+      <c r="G48">
+        <v>0.24990000000000001</v>
+      </c>
+      <c r="H48">
+        <v>0.25169999999999998</v>
+      </c>
+      <c r="I48">
+        <v>2020</v>
+      </c>
+      <c r="J48">
+        <v>0.91</v>
+      </c>
+      <c r="K48">
+        <v>5.23</v>
+      </c>
+      <c r="L48">
+        <v>6.26</v>
+      </c>
+      <c r="M48">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>14</v>
       </c>
-      <c r="C48" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" t="s">
-        <v>28</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="C49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" t="s">
         <v>93</v>
       </c>
-      <c r="F48">
+      <c r="F49">
         <v>0.27216000000000001</v>
       </c>
-      <c r="G48">
+      <c r="G49">
         <v>0.20351</v>
       </c>
-      <c r="H48">
+      <c r="H49">
         <v>0.20685999999999999</v>
       </c>
-      <c r="I48">
+      <c r="I49">
         <v>2006</v>
       </c>
-      <c r="J48">
-        <v>0</v>
-      </c>
-      <c r="K48">
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
         <v>3.6</v>
       </c>
-      <c r="L48">
+      <c r="L49">
         <v>3.38</v>
       </c>
-      <c r="M48">
+      <c r="M49">
         <v>4.16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>94</v>
-      </c>
-      <c r="B49" t="s">
-        <v>27</v>
-      </c>
-      <c r="C49" t="s">
-        <v>15</v>
-      </c>
-      <c r="D49" t="s">
-        <v>28</v>
-      </c>
-      <c r="E49" t="s">
-        <v>29</v>
-      </c>
-      <c r="F49">
-        <v>0.28100000000000003</v>
-      </c>
-      <c r="G49">
-        <v>0.22600000000000001</v>
-      </c>
-      <c r="H49">
-        <v>0.22600000000000001</v>
-      </c>
-      <c r="I49">
-        <v>1999</v>
-      </c>
-      <c r="J49">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="K49">
-        <v>15.55</v>
-      </c>
-      <c r="M49">
-        <v>12.37</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>95</v>
+        <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="C50" t="s">
         <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="E50" t="s">
-        <v>96</v>
-      </c>
-      <c r="F50">
-        <v>0.21190000000000001</v>
+        <v>17</v>
       </c>
       <c r="G50">
-        <v>0.1656</v>
+        <v>0.192</v>
       </c>
       <c r="H50">
-        <v>0.16800000000000001</v>
+        <v>0.192</v>
       </c>
       <c r="I50">
-        <v>2012</v>
+        <v>1997</v>
       </c>
       <c r="J50">
         <v>0</v>
       </c>
       <c r="K50">
-        <v>5.92</v>
+        <v>5.29</v>
       </c>
       <c r="L50">
-        <v>4.8600000000000003</v>
+        <v>1.42</v>
       </c>
       <c r="M50">
-        <v>2.5099999999999998</v>
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>14</v>
       </c>
       <c r="C51" t="s">
         <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
       <c r="E51" t="s">
-        <v>100</v>
-      </c>
-      <c r="F51">
-        <v>0.2707</v>
+        <v>17</v>
       </c>
       <c r="G51">
-        <v>0.22009999999999999</v>
+        <v>0.192</v>
       </c>
       <c r="H51">
-        <v>0.2228</v>
+        <v>0.192</v>
       </c>
       <c r="I51">
-        <v>2014</v>
+        <v>1997</v>
       </c>
       <c r="J51">
-        <v>0.37</v>
+        <v>0</v>
       </c>
       <c r="K51">
-        <v>15.69</v>
+        <v>5.64</v>
       </c>
       <c r="L51">
-        <v>2.36</v>
+        <v>3.32</v>
       </c>
       <c r="M51">
-        <v>4.75</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="B52" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>103</v>
+        <v>16</v>
       </c>
       <c r="E52" t="s">
-        <v>100</v>
-      </c>
-      <c r="F52">
-        <v>0.3044</v>
+        <v>17</v>
       </c>
       <c r="G52">
-        <v>0.24779999999999999</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="H52">
-        <v>0.25040000000000001</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="I52">
-        <v>2014</v>
+        <v>1997</v>
       </c>
       <c r="J52">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="K52">
-        <v>28.25</v>
+        <v>4.5</v>
       </c>
       <c r="L52">
-        <v>0.38</v>
+        <v>3.79</v>
       </c>
       <c r="M52">
-        <v>14.77</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="C53" t="s">
         <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E53" t="s">
-        <v>106</v>
-      </c>
-      <c r="F53">
-        <v>0.24610000000000001</v>
+        <v>17</v>
       </c>
       <c r="G53">
-        <v>0.20449999999999999</v>
+        <v>0.192</v>
       </c>
       <c r="H53">
-        <v>0.2064</v>
+        <v>0.192</v>
       </c>
       <c r="I53">
-        <v>2012</v>
+        <v>1997</v>
       </c>
       <c r="J53">
-        <v>0</v>
+        <v>0.49</v>
       </c>
       <c r="K53">
-        <v>3.49</v>
+        <v>8.65</v>
       </c>
       <c r="L53">
-        <v>4.63</v>
+        <v>0.95</v>
       </c>
       <c r="M53">
-        <v>0</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="C54" t="s">
         <v>15</v>
@@ -2730,121 +2763,109 @@
         <v>28</v>
       </c>
       <c r="E54" t="s">
-        <v>106</v>
-      </c>
-      <c r="F54">
-        <v>0.24510000000000001</v>
+        <v>39</v>
       </c>
       <c r="G54">
-        <v>0.20519999999999999</v>
+        <v>0.156</v>
       </c>
       <c r="H54">
-        <v>0.2072</v>
+        <v>0.156</v>
       </c>
       <c r="I54">
-        <v>2012</v>
+        <v>2003</v>
       </c>
       <c r="J54">
         <v>0</v>
       </c>
       <c r="K54">
-        <v>2.9</v>
-      </c>
-      <c r="L54">
-        <v>7.41</v>
+        <v>13.36</v>
       </c>
       <c r="M54">
-        <v>0</v>
+        <v>7.53</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="C55" t="s">
         <v>15</v>
       </c>
       <c r="D55" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E55" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="F55">
-        <v>0.2303</v>
+        <v>0.24746000000000001</v>
       </c>
       <c r="G55">
-        <v>0.1981</v>
+        <v>0.19312000000000001</v>
       </c>
       <c r="H55">
-        <v>0.1996</v>
+        <v>0.19585</v>
       </c>
       <c r="I55">
-        <v>2012</v>
+        <v>2005</v>
       </c>
       <c r="J55">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="K55">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="L55">
-        <v>6.48</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="M55">
-        <v>0</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>109</v>
+      <c r="A56" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="B56" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="C56" t="s">
         <v>15</v>
       </c>
       <c r="D56" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E56" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F56">
-        <v>0.1925</v>
+        <v>0.24611</v>
       </c>
       <c r="G56">
-        <v>0.1391</v>
+        <v>0.19616</v>
       </c>
       <c r="H56">
-        <v>0.14449999999999999</v>
-      </c>
-      <c r="I56">
-        <v>2013</v>
+        <v>0.19868</v>
       </c>
       <c r="J56">
         <v>0</v>
       </c>
       <c r="K56">
-        <v>2.77</v>
+        <v>11.38</v>
       </c>
       <c r="L56">
-        <v>2.46</v>
+        <v>3.58</v>
       </c>
       <c r="M56">
-        <v>0</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B57" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="C57" t="s">
         <v>15</v>
@@ -2853,36 +2874,39 @@
         <v>28</v>
       </c>
       <c r="E57" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="F57">
-        <v>0.24611</v>
+        <v>0.22819999999999999</v>
       </c>
       <c r="G57">
-        <v>0.19616</v>
+        <v>0.193</v>
       </c>
       <c r="H57">
-        <v>0.19868</v>
+        <v>0.19470000000000001</v>
+      </c>
+      <c r="I57">
+        <v>2019</v>
       </c>
       <c r="J57">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="K57">
-        <v>11.38</v>
+        <v>3.87</v>
       </c>
       <c r="L57">
-        <v>3.58</v>
+        <v>11.76</v>
       </c>
       <c r="M57">
-        <v>5.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>113</v>
+        <v>23</v>
       </c>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="C58" t="s">
         <v>15</v>
@@ -2891,39 +2915,36 @@
         <v>16</v>
       </c>
       <c r="E58" t="s">
-        <v>82</v>
-      </c>
-      <c r="F58">
-        <v>0.25369999999999998</v>
+        <v>17</v>
       </c>
       <c r="G58">
-        <v>0.21029999999999999</v>
+        <v>0.186</v>
       </c>
       <c r="H58">
-        <v>0.21240000000000001</v>
+        <v>0.186</v>
       </c>
       <c r="I58">
-        <v>2014</v>
+        <v>1997</v>
       </c>
       <c r="J58">
-        <v>0.19</v>
+        <v>0</v>
       </c>
       <c r="K58">
-        <v>7.28</v>
+        <v>5.96</v>
       </c>
       <c r="L58">
-        <v>6.04</v>
+        <v>1.9</v>
       </c>
       <c r="M58">
-        <v>6.74</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="B59" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="C59" t="s">
         <v>15</v>
@@ -2935,74 +2956,65 @@
         <v>82</v>
       </c>
       <c r="F59">
-        <v>0.27629999999999999</v>
+        <v>0.25209999999999999</v>
       </c>
       <c r="G59">
-        <v>0.20649999999999999</v>
+        <v>0.17510000000000001</v>
       </c>
       <c r="H59">
-        <v>0.21329999999999999</v>
-      </c>
-      <c r="I59">
-        <v>2014</v>
+        <v>0.17929999999999999</v>
       </c>
       <c r="J59">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="K59">
-        <v>19.45</v>
+        <v>5.6</v>
       </c>
       <c r="L59">
-        <v>2.85</v>
+        <v>2.9</v>
       </c>
       <c r="M59">
-        <v>12.64</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="B60" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="C60" t="s">
         <v>15</v>
       </c>
       <c r="D60" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E60" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F60">
-        <v>0.26550000000000001</v>
+        <v>0.27700000000000002</v>
       </c>
       <c r="G60">
-        <v>0.2079</v>
-      </c>
-      <c r="H60">
-        <v>0.2109</v>
+        <v>0.158</v>
       </c>
       <c r="I60">
-        <v>2014</v>
+        <v>2006</v>
       </c>
       <c r="J60">
-        <v>1.1499999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="K60">
-        <v>14.32</v>
-      </c>
-      <c r="L60">
-        <v>11.7</v>
+        <v>18.739999999999998</v>
       </c>
       <c r="M60">
-        <v>10.43</v>
+        <v>4.09</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B61" t="s">
         <v>117</v>
@@ -3043,51 +3055,51 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B62" t="s">
-        <v>24</v>
+        <v>117</v>
       </c>
       <c r="C62" t="s">
         <v>15</v>
       </c>
       <c r="D62" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E62" t="s">
         <v>82</v>
       </c>
       <c r="F62">
-        <v>0.22819999999999999</v>
+        <v>0.26550000000000001</v>
       </c>
       <c r="G62">
-        <v>0.193</v>
+        <v>0.2079</v>
       </c>
       <c r="H62">
-        <v>0.19470000000000001</v>
+        <v>0.2109</v>
       </c>
       <c r="I62">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="J62">
-        <v>0.4</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="K62">
-        <v>3.87</v>
+        <v>14.32</v>
       </c>
       <c r="L62">
-        <v>11.76</v>
+        <v>11.7</v>
       </c>
       <c r="M62">
-        <v>0</v>
+        <v>10.43</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B63" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="C63" t="s">
         <v>15</v>
@@ -3096,121 +3108,121 @@
         <v>16</v>
       </c>
       <c r="E63" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="F63">
-        <v>0.22625999999999999</v>
+        <v>0.27629999999999999</v>
       </c>
       <c r="G63">
-        <v>0.18717</v>
+        <v>0.20649999999999999</v>
       </c>
       <c r="H63">
-        <v>0.18912000000000001</v>
+        <v>0.21329999999999999</v>
       </c>
       <c r="I63">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="J63">
-        <v>2.08</v>
+        <v>0.97</v>
       </c>
       <c r="K63">
-        <v>4.42</v>
+        <v>19.45</v>
       </c>
       <c r="L63">
-        <v>8.11</v>
+        <v>2.85</v>
       </c>
       <c r="M63">
-        <v>2.34</v>
+        <v>12.64</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="B64" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="C64" t="s">
         <v>15</v>
       </c>
       <c r="D64" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="E64" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="F64">
-        <v>0.28489999999999999</v>
+        <v>0.2707</v>
       </c>
       <c r="G64">
-        <v>0.24990000000000001</v>
+        <v>0.22009999999999999</v>
       </c>
       <c r="H64">
-        <v>0.25169999999999998</v>
+        <v>0.2228</v>
       </c>
       <c r="I64">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="J64">
-        <v>0.91</v>
+        <v>0.37</v>
       </c>
       <c r="K64">
-        <v>5.23</v>
+        <v>15.69</v>
       </c>
       <c r="L64">
-        <v>6.26</v>
+        <v>2.36</v>
       </c>
       <c r="M64">
-        <v>1.25</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B65" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="C65" t="s">
         <v>15</v>
       </c>
       <c r="D65" t="s">
-        <v>125</v>
+        <v>16</v>
       </c>
       <c r="E65" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="F65">
-        <v>0.23860000000000001</v>
+        <v>0.2702</v>
       </c>
       <c r="G65">
-        <v>0.18429999999999999</v>
+        <v>0.21840000000000001</v>
       </c>
       <c r="H65">
-        <v>0.187</v>
+        <v>0.22370000000000001</v>
       </c>
       <c r="I65">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="J65">
         <v>0</v>
       </c>
       <c r="K65">
-        <v>3.96</v>
+        <v>5.26</v>
       </c>
       <c r="L65">
-        <v>2.14</v>
+        <v>0</v>
       </c>
       <c r="M65">
-        <v>1.21</v>
+        <v>4.5199999999999996</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>127</v>
+        <v>35</v>
       </c>
       <c r="B66" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C66" t="s">
         <v>15</v>
@@ -3219,39 +3231,36 @@
         <v>28</v>
       </c>
       <c r="E66" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="F66">
-        <v>0.21329999999999999</v>
+        <v>0.29399999999999998</v>
       </c>
       <c r="G66">
-        <v>0.18</v>
-      </c>
-      <c r="H66">
-        <v>0.18179999999999999</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="I66">
-        <v>2021</v>
+        <v>2002</v>
       </c>
       <c r="J66">
-        <v>0</v>
+        <v>2.46</v>
       </c>
       <c r="K66">
-        <v>0.9</v>
+        <v>27.08</v>
       </c>
       <c r="L66">
-        <v>6.57</v>
+        <v>5.79</v>
       </c>
       <c r="M66">
-        <v>0.84</v>
+        <v>10.59</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="B67" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="C67" t="s">
         <v>15</v>
@@ -3263,70 +3272,74 @@
         <v>82</v>
       </c>
       <c r="F67">
-        <v>0.25209999999999999</v>
+        <v>0.31322</v>
       </c>
       <c r="G67">
-        <v>0.17510000000000001</v>
+        <v>0.21704000000000001</v>
       </c>
       <c r="H67">
-        <v>0.17929999999999999</v>
+        <v>0.22187000000000001</v>
+      </c>
+      <c r="I67">
+        <v>2005</v>
       </c>
       <c r="J67">
-        <v>0.98</v>
+        <v>2.14</v>
       </c>
       <c r="K67">
-        <v>5.6</v>
-      </c>
-      <c r="L67">
-        <v>2.9</v>
+        <v>9.17</v>
       </c>
       <c r="M67">
-        <v>2.46</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="B68" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="C68" t="s">
         <v>15</v>
       </c>
       <c r="D68" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="E68" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="F68">
-        <v>0.2702</v>
+        <v>0.3044</v>
       </c>
       <c r="G68">
-        <v>0.21840000000000001</v>
+        <v>0.24779999999999999</v>
       </c>
       <c r="H68">
-        <v>0.22370000000000001</v>
+        <v>0.25040000000000001</v>
       </c>
       <c r="I68">
-        <v>2022</v>
+        <v>2014</v>
       </c>
       <c r="J68">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="K68">
-        <v>5.26</v>
+        <v>28.25</v>
       </c>
       <c r="L68">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="M68">
-        <v>4.5199999999999996</v>
+        <v>14.77</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:M1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M68">
+      <sortCondition ref="B1:B68"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>